<commit_message>
Sync BOP and Package runners: hidden terminals, grouped logs, robust DateTime handling, and exit code fixes
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-29.xlsx
+++ b/WB_Test_Report_2025-12-29.xlsx
@@ -4,11 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Package_1" sheetId="2" r:id="rId2"/>
-    <sheet name="Package_2" sheetId="3" r:id="rId3"/>
-    <sheet name="Package_3" sheetId="4" r:id="rId4"/>
-    <sheet name="Package_4" sheetId="5" r:id="rId5"/>
-    <sheet name="Package_5" sheetId="6" r:id="rId6"/>
+    <sheet name="BOP_1" sheetId="2" r:id="rId2"/>
+    <sheet name="BOP_2" sheetId="3" r:id="rId3"/>
+    <sheet name="BOP_3" sheetId="4" r:id="rId4"/>
+    <sheet name="BOP_4" sheetId="5" r:id="rId5"/>
+    <sheet name="BOP_5" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -435,22 +435,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Package (OH)</v>
+        <v>BOP (PA)</v>
       </c>
       <c r="C2" t="str">
-        <v>3003179903</v>
+        <v>3003179993</v>
       </c>
       <c r="D2" t="str">
-        <v>1003052821</v>
+        <v>N/A</v>
       </c>
       <c r="E2" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>846.87</v>
+        <v>94.20</v>
       </c>
       <c r="G2" t="str">
-        <v>OH</v>
+        <v>PA</v>
       </c>
     </row>
     <row r="3">
@@ -458,10 +458,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>Package (PA)</v>
+        <v>BOP (MI)</v>
       </c>
       <c r="C3" t="str">
-        <v>3003179908</v>
+        <v>3003180002</v>
       </c>
       <c r="D3" t="str">
         <v>N/A</v>
@@ -470,10 +470,10 @@
         <v>FAILED</v>
       </c>
       <c r="F3" t="str">
-        <v>144.12</v>
+        <v>152.70</v>
       </c>
       <c r="G3" t="str">
-        <v>PA</v>
+        <v>MI</v>
       </c>
     </row>
     <row r="4">
@@ -481,22 +481,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>Package (MI)</v>
+        <v>BOP (OH)</v>
       </c>
       <c r="C4" t="str">
-        <v>3003179909</v>
+        <v>3003180003</v>
       </c>
       <c r="D4" t="str">
-        <v>1003052823</v>
+        <v>N/A</v>
       </c>
       <c r="E4" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F4" t="str">
-        <v>862.75</v>
+        <v>157.41</v>
       </c>
       <c r="G4" t="str">
-        <v>MI</v>
+        <v>OH</v>
       </c>
     </row>
     <row r="5">
@@ -504,10 +504,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>Package (WI)</v>
+        <v>BOP (DE)</v>
       </c>
       <c r="C5" t="str">
-        <v>3003179912</v>
+        <v>3003180004</v>
       </c>
       <c r="D5" t="str">
         <v>N/A</v>
@@ -516,10 +516,10 @@
         <v>FAILED</v>
       </c>
       <c r="F5" t="str">
-        <v>444.42</v>
+        <v>258.13</v>
       </c>
       <c r="G5" t="str">
-        <v>WI</v>
+        <v>DE</v>
       </c>
     </row>
     <row r="6">
@@ -527,22 +527,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>Package (DE)</v>
+        <v>BOP (WI)</v>
       </c>
       <c r="C6" t="str">
-        <v>3003179914</v>
+        <v>3003180005</v>
       </c>
       <c r="D6" t="str">
-        <v>1003052824</v>
+        <v>1003052850</v>
       </c>
       <c r="E6" t="str">
         <v>PASSED</v>
       </c>
       <c r="F6" t="str">
-        <v>792.93</v>
+        <v>462.40</v>
       </c>
       <c r="G6" t="str">
-        <v>DE</v>
+        <v>WI</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +554,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -572,143 +572,79 @@
       <c r="D1" t="str">
         <v>Timestamp</v>
       </c>
+      <c r="E1" t="str">
+        <v>Parallel Jobs at Start</v>
+      </c>
+      <c r="F1" t="str">
+        <v>CPU at Start</v>
+      </c>
+      <c r="G1" t="str">
+        <v>RAM at Start</v>
+      </c>
+      <c r="H1" t="str">
+        <v>CPU at End</v>
+      </c>
+      <c r="I1" t="str">
+        <v>RAM at End</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Retry Count</v>
+      </c>
+      <c r="K1" t="str">
+        <v>HTTP Timings</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Network Errors</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Account Created</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B2" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C2" t="str">
-        <v>73.71s</v>
+        <v>94.20s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-29T13:32:12.464Z</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Commercial Property Package Completed</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C3" t="str">
-        <v>315.11s</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2025-12-29T13:37:27.580Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>General Liability Completed</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>94.81s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-29T13:39:02.388Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Inland Marine Completed</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>38.73s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-29T13:39:41.120Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Crime Completed</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>22.93s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-29T13:40:04.049Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>60.20s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-29T13:41:04.253Z</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B8" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C8" t="str">
-        <v>38.88s</v>
-      </c>
-      <c r="D8" t="str">
-        <v>2025-12-29T13:41:43.136Z</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B9" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C9" t="str">
-        <v>48.71s</v>
-      </c>
-      <c r="D9" t="str">
-        <v>2025-12-29T13:42:31.849Z</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B10" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C10" t="str">
-        <v>153.79s</v>
-      </c>
-      <c r="D10" t="str">
-        <v>2025-12-29T13:45:05.640Z</v>
+        <v>2025-12-29T23:40:03.785Z</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -726,6 +662,30 @@
       <c r="D1" t="str">
         <v>Timestamp</v>
       </c>
+      <c r="E1" t="str">
+        <v>Parallel Jobs at Start</v>
+      </c>
+      <c r="F1" t="str">
+        <v>CPU at Start</v>
+      </c>
+      <c r="G1" t="str">
+        <v>RAM at Start</v>
+      </c>
+      <c r="H1" t="str">
+        <v>CPU at End</v>
+      </c>
+      <c r="I1" t="str">
+        <v>RAM at End</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Retry Count</v>
+      </c>
+      <c r="K1" t="str">
+        <v>HTTP Timings</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Network Errors</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -735,10 +695,34 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>73.41s</v>
+        <v>70.08s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-29T13:46:14.085Z</v>
+        <v>2025-12-29T23:41:20.832Z</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -749,22 +733,22 @@
         <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>70.71s</v>
+        <v>82.62s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-29T13:47:24.796Z</v>
+        <v>2025-12-29T23:42:43.451Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -782,6 +766,30 @@
       <c r="D1" t="str">
         <v>Timestamp</v>
       </c>
+      <c r="E1" t="str">
+        <v>Parallel Jobs at Start</v>
+      </c>
+      <c r="F1" t="str">
+        <v>CPU at Start</v>
+      </c>
+      <c r="G1" t="str">
+        <v>RAM at Start</v>
+      </c>
+      <c r="H1" t="str">
+        <v>CPU at End</v>
+      </c>
+      <c r="I1" t="str">
+        <v>RAM at End</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Retry Count</v>
+      </c>
+      <c r="K1" t="str">
+        <v>HTTP Timings</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Network Errors</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -791,134 +799,60 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>73.67s</v>
+        <v>74.28s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-29T13:48:44.522Z</v>
+        <v>2025-12-29T23:41:24.884Z</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Commercial Property Package Completed</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>298.25s</v>
+        <v>83.13s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-29T13:53:42.778Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>General Liability Completed</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>98.42s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-29T13:55:21.199Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Inland Marine Completed</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>39.22s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-29T13:56:00.422Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Crime Completed</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>23.03s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-29T13:56:23.454Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>84.93s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-29T13:57:48.388Z</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B8" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C8" t="str">
-        <v>35.46s</v>
-      </c>
-      <c r="D8" t="str">
-        <v>2025-12-29T13:58:23.849Z</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B9" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C9" t="str">
-        <v>55.18s</v>
-      </c>
-      <c r="D9" t="str">
-        <v>2025-12-29T13:59:19.034Z</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B10" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C10" t="str">
-        <v>154.59s</v>
-      </c>
-      <c r="D10" t="str">
-        <v>2025-12-29T14:01:53.625Z</v>
+        <v>2025-12-29T23:42:48.019Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -936,6 +870,30 @@
       <c r="D1" t="str">
         <v>Timestamp</v>
       </c>
+      <c r="E1" t="str">
+        <v>Parallel Jobs at Start</v>
+      </c>
+      <c r="F1" t="str">
+        <v>CPU at Start</v>
+      </c>
+      <c r="G1" t="str">
+        <v>RAM at Start</v>
+      </c>
+      <c r="H1" t="str">
+        <v>CPU at End</v>
+      </c>
+      <c r="I1" t="str">
+        <v>RAM at End</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Retry Count</v>
+      </c>
+      <c r="K1" t="str">
+        <v>HTTP Timings</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Network Errors</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -945,50 +903,60 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>71.68s</v>
+        <v>70.03s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-29T14:02:23.609Z</v>
+        <v>2025-12-29T23:44:05.056Z</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Commercial Property Package Completed</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>287.14s</v>
+        <v>188.10s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-29T14:07:10.751Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B4" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>85.60s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-29T14:08:36.352Z</v>
+        <v>2025-12-29T23:47:13.160Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1006,6 +974,30 @@
       <c r="D1" t="str">
         <v>Timestamp</v>
       </c>
+      <c r="E1" t="str">
+        <v>Parallel Jobs at Start</v>
+      </c>
+      <c r="F1" t="str">
+        <v>CPU at Start</v>
+      </c>
+      <c r="G1" t="str">
+        <v>RAM at Start</v>
+      </c>
+      <c r="H1" t="str">
+        <v>CPU at End</v>
+      </c>
+      <c r="I1" t="str">
+        <v>RAM at End</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Retry Count</v>
+      </c>
+      <c r="K1" t="str">
+        <v>HTTP Timings</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Network Errors</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1015,127 +1007,109 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>71.20s</v>
+        <v>70.83s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-29T14:09:52.573Z</v>
+        <v>2025-12-29T23:48:32.314Z</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Commercial Property Package Completed</v>
+        <v>Building and Classification Added</v>
       </c>
       <c r="B3" t="str">
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>282.01s</v>
+        <v>138.27s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-29T14:14:34.588Z</v>
+        <v>2025-12-29T23:50:50.586Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>General Liability Completed</v>
+        <v>Quote Rated Successfully</v>
       </c>
       <c r="B4" t="str">
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>82.25s</v>
+        <v>22.12s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-29T14:15:56.844Z</v>
+        <v>2025-12-29T23:51:12.704Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Inland Marine Completed</v>
+        <v>Submitting for Approval</v>
       </c>
       <c r="B5" t="str">
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>37.22s</v>
+        <v>36.93s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-29T14:16:34.062Z</v>
+        <v>2025-12-29T23:51:49.638Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Crime Completed</v>
+        <v>UW Issues Approved in PolicyCenter</v>
       </c>
       <c r="B6" t="str">
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>22.13s</v>
+        <v>43.67s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-29T14:16:56.189Z</v>
+        <v>2025-12-29T23:52:33.311Z</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Quote Rated Successfully</v>
+        <v>Policy Issued Successfully</v>
       </c>
       <c r="B7" t="str">
         <v>PASSED</v>
       </c>
       <c r="C7" t="str">
-        <v>60.30s</v>
+        <v>150.58s</v>
       </c>
       <c r="D7" t="str">
-        <v>2025-12-29T14:17:56.492Z</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B8" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C8" t="str">
-        <v>36.58s</v>
-      </c>
-      <c r="D8" t="str">
-        <v>2025-12-29T14:18:33.072Z</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B9" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C9" t="str">
-        <v>50.38s</v>
-      </c>
-      <c r="D9" t="str">
-        <v>2025-12-29T14:19:23.455Z</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B10" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C10" t="str">
-        <v>150.86s</v>
-      </c>
-      <c r="D10" t="str">
-        <v>2025-12-29T14:21:54.319Z</v>
+        <v>2025-12-29T23:55:03.896Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>